<commit_message>
Removed abbreviation translation in extractEntsTBI
</commit_message>
<xml_diff>
--- a/test/test_fmt.xlsx
+++ b/test/test_fmt.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ualbertaca-my.sharepoint.com/personal/hqiu1_ualberta_ca/Documents/Coding/NLP Tools/test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_14A177A88710560EDB1A3411595ED876568C40BF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3CBDA793-97E7-4577-8E2D-6BA49AD49487}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="11_14A177A88710560EDB1A3411595ED876568C40BF" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8FD7F0EB-9E4D-4F68-B43B-E03B8CA857CC}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="10690" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="165">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="161">
   <si>
     <t>Unnamed: 0.1</t>
   </si>
@@ -347,31 +347,6 @@
   </si>
   <si>
     <t>[[" Preinjury depressive symptoms ", " Affective and behavioral problems ", " 177 "], [" Preinjury depressive symptoms ", " Cognitive problems ", " 177 "], [" Preinjury depressive symptoms ", " Mental health-related quality-of-life ", " 177 "]]</t>
-  </si>
-  <si>
-    <t>Long-term outcome in elderly patients after operation for traumatic intracranial hemorrhage.</t>
-  </si>
-  <si>
-    <t>OBJECTIVE: This study examined outcomes in elderly TBI patients who underwent a cranial operation., METHODS: We identified TBI patients &gt; or = 65 who underwent a cranial operation from January 1, 2004 to December 31, 2008. Data collected included: age, admission GCS, mechanism of injury, ISS, Head AIS, type of operation, hemorrhage acuity, time to operation, pre-hospital warfarin or clopidogrel, and in-hospital death. Survivors were contacted by phone to determine an Extended Glasgow Outcome Score (GOSE). A favorable outcome was defined as having a GOSE of &gt; or = 5 at follow-up, an unfavorable outcome was defined as: in-hospital death, death within one year of injury, and a GOSE &lt; 5 at follow-up. Chi-square and student's t-test were used., RESULTS: One hundred sixty-four elderly TBI patients underwent cranial surgery. Mean age was 79.2 +/- 7.6 years. Most patients: had a ground level fall (86.0%), suffered a subdural hematoma (95.1%), and underwent craniotomy (89.0%). Twenty-eight percent died in the hospital and another 20.1% died within one year. Fifty-six patients were eligible for a GOSE interview of these: 17 were lost to follow-up, seven refused the GOSE interview, 22 had a GOSE &gt; or = 5, and ten had a GOSE &lt; 5. Mean follow-up was 42.6 +/- 14.9 months. Of all the factors analyzed, only older age was associated with an unfavorable outcome., CONCLUSIONS: While age was associated with outcome, we were unable to demonstrate any other early factors that were associated with long-term functional outcome in elderly patients that underwent a cranial operation for TBI.</t>
-  </si>
-  <si>
-    <t>{
-  "choices": [
-    {
-      "finish_reason": "stop",
-      "index": 0,
-      "logprobs": null,
-      "text": "\n| --- | --- | --- |\n| Age | Unfavorable outcome | 164 |\n| Admission GCS |  | 164 |\n| Mechanism of injury |  | 164 |\n| ISS |  | 164 |\n| Head AIS |  | 164 |\n| Type of operation |  | 164 |\n| Hemorrhage acuity |  | 164 |\n| Time to operation |  | 164 |\n| Pre-hospital warfarin or clopidogrel |  | 164 |\n| In-hospital death |  | 164 |"
-    }
-  ],
-  "created": 1654226850,
-  "id": "cmpl-5EsGAme2rGmM4I8aMgaiq1GsMWiuT",
-  "model": "text-davinci-002",
-  "object": "text_completion"
-}</t>
-  </si>
-  <si>
-    <t>[[" Age ", " Unfavorable outcome ", " 164 "], [" Admission GCS ", "  ", " 164 "], [" Mechanism of injury ", "  ", " 164 "], [" ISS ", "  ", " 164 "], [" Head AIS ", "  ", " 164 "], [" Type of operation ", "  ", " 164 "], [" Hemorrhage acuity ", "  ", " 164 "], [" Time to operation ", "  ", " 164 "], [" Pre-hospital warfarin or clopidogrel ", "  ", " 164 "], [" In-hospital death ", "  ", " 164 "]]</t>
   </si>
   <si>
     <t>A systematic review of age and gender factors in prolonged post-concussion symptoms after mild head injury.</t>
@@ -1386,8 +1361,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H40"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K36" sqref="K36"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="M23" sqref="M23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1709,29 +1684,6 @@
         <v>56</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14">
-        <v>7</v>
-      </c>
-      <c r="B14">
-        <v>7</v>
-      </c>
-      <c r="D14" t="s">
-        <v>57</v>
-      </c>
-      <c r="E14" t="s">
-        <v>58</v>
-      </c>
-      <c r="F14" t="s">
-        <v>10</v>
-      </c>
-      <c r="G14" t="s">
-        <v>59</v>
-      </c>
-      <c r="H14" t="s">
-        <v>60</v>
-      </c>
-    </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>8</v>
@@ -1740,19 +1692,19 @@
         <v>8</v>
       </c>
       <c r="D15" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="E15" t="s">
-        <v>62</v>
+        <v>58</v>
       </c>
       <c r="F15" t="s">
         <v>10</v>
       </c>
       <c r="G15" t="s">
-        <v>63</v>
+        <v>59</v>
       </c>
       <c r="H15" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
@@ -1763,19 +1715,19 @@
         <v>9</v>
       </c>
       <c r="D16" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="E16" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="F16" t="s">
         <v>10</v>
       </c>
       <c r="G16" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="H16" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
@@ -1786,19 +1738,19 @@
         <v>10</v>
       </c>
       <c r="D17" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="E17" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="F17" t="s">
         <v>10</v>
       </c>
       <c r="G17" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="H17" t="s">
-        <v>72</v>
+        <v>68</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
@@ -1809,19 +1761,19 @@
         <v>11</v>
       </c>
       <c r="D18" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="E18" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F18" t="s">
         <v>10</v>
       </c>
       <c r="G18" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="H18" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
@@ -1832,19 +1784,19 @@
         <v>12</v>
       </c>
       <c r="D19" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E19" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="F19" t="s">
         <v>10</v>
       </c>
       <c r="G19" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="H19" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
@@ -1855,19 +1807,19 @@
         <v>13</v>
       </c>
       <c r="D20" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E20" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="F20" t="s">
         <v>10</v>
       </c>
       <c r="G20" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="H20" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
@@ -1878,19 +1830,19 @@
         <v>14</v>
       </c>
       <c r="D21" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E21" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="F21" t="s">
         <v>10</v>
       </c>
       <c r="G21" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="H21" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.3">
@@ -1901,19 +1853,19 @@
         <v>15</v>
       </c>
       <c r="D22" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E22" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="F22" t="s">
         <v>10</v>
       </c>
       <c r="G22" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="H22" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.3">
@@ -1924,19 +1876,19 @@
         <v>16</v>
       </c>
       <c r="D23" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E23" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="F23" t="s">
         <v>10</v>
       </c>
       <c r="G23" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="H23" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.3">
@@ -1947,19 +1899,19 @@
         <v>17</v>
       </c>
       <c r="D24" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E24" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="F24" t="s">
         <v>10</v>
       </c>
       <c r="G24" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="H24" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.3">
@@ -1970,19 +1922,19 @@
         <v>18</v>
       </c>
       <c r="D25" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="E25" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="F25" t="s">
         <v>10</v>
       </c>
       <c r="G25" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="H25" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.3">
@@ -1993,19 +1945,19 @@
         <v>19</v>
       </c>
       <c r="D26" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E26" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="F26" t="s">
         <v>10</v>
       </c>
       <c r="G26" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="H26" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.3">
@@ -2016,19 +1968,19 @@
         <v>20</v>
       </c>
       <c r="D27" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E27" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="F27" t="s">
         <v>10</v>
       </c>
       <c r="G27" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="H27" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.3">
@@ -2039,19 +1991,19 @@
         <v>21</v>
       </c>
       <c r="D28" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E28" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="F28" t="s">
         <v>10</v>
       </c>
       <c r="G28" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="H28" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.3">
@@ -2062,19 +2014,19 @@
         <v>22</v>
       </c>
       <c r="D29" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E29" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="F29" t="s">
         <v>10</v>
       </c>
       <c r="G29" t="s">
-        <v>119</v>
+        <v>115</v>
       </c>
       <c r="H29" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.3">
@@ -2085,19 +2037,19 @@
         <v>23</v>
       </c>
       <c r="D30" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="E30" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="F30" t="s">
         <v>10</v>
       </c>
       <c r="G30" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="H30" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.3">
@@ -2108,19 +2060,19 @@
         <v>24</v>
       </c>
       <c r="D31" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E31" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="F31" t="s">
         <v>10</v>
       </c>
       <c r="G31" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="H31" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.3">
@@ -2131,19 +2083,19 @@
         <v>25</v>
       </c>
       <c r="D32" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E32" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="F32" t="s">
         <v>10</v>
       </c>
       <c r="G32" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="H32" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.3">
@@ -2154,19 +2106,19 @@
         <v>26</v>
       </c>
       <c r="D33" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="E33" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="F33" t="s">
         <v>10</v>
       </c>
       <c r="G33" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="H33" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.3">
@@ -2177,19 +2129,19 @@
         <v>27</v>
       </c>
       <c r="D34" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="E34" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="F34" t="s">
         <v>10</v>
       </c>
       <c r="G34" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="H34" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.3">
@@ -2200,19 +2152,19 @@
         <v>28</v>
       </c>
       <c r="D35" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="E35" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="F35" t="s">
         <v>10</v>
       </c>
       <c r="G35" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="H35" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.3">
@@ -2223,19 +2175,19 @@
         <v>29</v>
       </c>
       <c r="D36" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
       <c r="E36" t="s">
-        <v>146</v>
+        <v>142</v>
       </c>
       <c r="F36" t="s">
         <v>10</v>
       </c>
       <c r="G36" t="s">
-        <v>147</v>
+        <v>143</v>
       </c>
       <c r="H36" t="s">
-        <v>148</v>
+        <v>144</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.3">
@@ -2246,19 +2198,19 @@
         <v>30</v>
       </c>
       <c r="D37" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="E37" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="F37" t="s">
         <v>10</v>
       </c>
       <c r="G37" t="s">
-        <v>151</v>
+        <v>147</v>
       </c>
       <c r="H37" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.3">
@@ -2269,19 +2221,19 @@
         <v>31</v>
       </c>
       <c r="D38" t="s">
-        <v>153</v>
+        <v>149</v>
       </c>
       <c r="E38" t="s">
-        <v>154</v>
+        <v>150</v>
       </c>
       <c r="F38" t="s">
         <v>10</v>
       </c>
       <c r="G38" t="s">
-        <v>155</v>
+        <v>151</v>
       </c>
       <c r="H38" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.3">
@@ -2292,19 +2244,19 @@
         <v>32</v>
       </c>
       <c r="D39" t="s">
-        <v>157</v>
+        <v>153</v>
       </c>
       <c r="E39" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="F39" t="s">
         <v>10</v>
       </c>
       <c r="G39" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="H39" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.3">
@@ -2315,19 +2267,19 @@
         <v>33</v>
       </c>
       <c r="D40" t="s">
-        <v>161</v>
+        <v>157</v>
       </c>
       <c r="E40" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="F40" t="s">
         <v>10</v>
       </c>
       <c r="G40" t="s">
-        <v>163</v>
+        <v>159</v>
       </c>
       <c r="H40" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>